<commit_message>
Made some tweaks to knn to improve speed
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -201,7 +201,7 @@
                   <c:v>6.56574481348E6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2435.18475369719</c:v>
+                  <c:v>2488.66572260652</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1271,7 +1271,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1293,7 +1293,7 @@
         <v>6565744.81348</v>
       </c>
       <c r="B2" s="1">
-        <v>2435.18475369719</v>
+        <v>2488.6657226065199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>